<commit_message>
Fixed the final data set additions to SFHP
</commit_message>
<xml_diff>
--- a/Data/2021-22 Teacher Data - All Teachers.xlsx
+++ b/Data/2021-22 Teacher Data - All Teachers.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5295f811bc7b9736/Documents/Career/Learning/Projects/Real Estate MA/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5295f811bc7b9736/Documents/MA-Where-To-Live-Application/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1FB64264-4E19-48A0-815E-E16E125A9245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{1FB64264-4E19-48A0-815E-E16E125A9245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D3121B4-DFBB-4FAE-B243-1A1C7F2C18B1}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="8670" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Teacher Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Teacher Data'!$A$2:$H$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Teacher Data'!$A$2:$H$403</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -5424,6 +5424,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:H403"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -5480,7 +5481,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -5506,7 +5507,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -5532,7 +5533,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
@@ -5558,7 +5559,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>33</v>
       </c>
@@ -5584,7 +5585,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>41</v>
       </c>
@@ -5610,7 +5611,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>48</v>
       </c>
@@ -5636,7 +5637,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>56</v>
       </c>
@@ -5662,7 +5663,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>62</v>
       </c>
@@ -5688,7 +5689,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>69</v>
       </c>
@@ -5714,7 +5715,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>76</v>
       </c>
@@ -5740,7 +5741,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>83</v>
       </c>
@@ -5766,7 +5767,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>91</v>
       </c>
@@ -5792,7 +5793,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>99</v>
       </c>
@@ -5818,7 +5819,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>107</v>
       </c>
@@ -5844,7 +5845,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>115</v>
       </c>
@@ -5870,7 +5871,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>122</v>
       </c>
@@ -5896,7 +5897,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>127</v>
       </c>
@@ -5922,7 +5923,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>133</v>
       </c>
@@ -5948,7 +5949,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>141</v>
       </c>
@@ -5974,7 +5975,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>148</v>
       </c>
@@ -6000,7 +6001,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>156</v>
       </c>
@@ -6026,7 +6027,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>162</v>
       </c>
@@ -6052,7 +6053,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>168</v>
       </c>
@@ -6078,7 +6079,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>174</v>
       </c>
@@ -6104,7 +6105,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>179</v>
       </c>
@@ -6130,7 +6131,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>186</v>
       </c>
@@ -6156,7 +6157,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>193</v>
       </c>
@@ -6182,7 +6183,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>197</v>
       </c>
@@ -6208,7 +6209,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>202</v>
       </c>
@@ -6234,7 +6235,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>209</v>
       </c>
@@ -6260,7 +6261,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>217</v>
       </c>
@@ -6286,7 +6287,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>223</v>
       </c>
@@ -6312,7 +6313,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>229</v>
       </c>
@@ -6338,7 +6339,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>237</v>
       </c>
@@ -6364,7 +6365,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>241</v>
       </c>
@@ -6390,7 +6391,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>246</v>
       </c>
@@ -6416,7 +6417,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>251</v>
       </c>
@@ -6442,7 +6443,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>256</v>
       </c>
@@ -6468,7 +6469,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>262</v>
       </c>
@@ -6494,7 +6495,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>268</v>
       </c>
@@ -6520,7 +6521,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>273</v>
       </c>
@@ -6546,7 +6547,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>281</v>
       </c>
@@ -6572,7 +6573,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>287</v>
       </c>
@@ -6598,7 +6599,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>293</v>
       </c>
@@ -6624,7 +6625,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>298</v>
       </c>
@@ -6650,7 +6651,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>303</v>
       </c>
@@ -6676,7 +6677,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>309</v>
       </c>
@@ -6702,7 +6703,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>315</v>
       </c>
@@ -6728,7 +6729,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>319</v>
       </c>
@@ -6754,7 +6755,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>325</v>
       </c>
@@ -6780,7 +6781,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>331</v>
       </c>
@@ -6806,7 +6807,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>337</v>
       </c>
@@ -6832,7 +6833,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>342</v>
       </c>
@@ -6858,7 +6859,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>345</v>
       </c>
@@ -6884,7 +6885,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>349</v>
       </c>
@@ -6910,7 +6911,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>355</v>
       </c>
@@ -6936,7 +6937,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>360</v>
       </c>
@@ -6962,7 +6963,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>367</v>
       </c>
@@ -6988,7 +6989,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>373</v>
       </c>
@@ -7014,7 +7015,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>376</v>
       </c>
@@ -7040,7 +7041,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>381</v>
       </c>
@@ -7066,7 +7067,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>386</v>
       </c>
@@ -7092,7 +7093,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>390</v>
       </c>
@@ -7118,7 +7119,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>395</v>
       </c>
@@ -7144,7 +7145,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>402</v>
       </c>
@@ -7170,7 +7171,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>407</v>
       </c>
@@ -7196,7 +7197,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>411</v>
       </c>
@@ -7222,7 +7223,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>416</v>
       </c>
@@ -7248,7 +7249,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>419</v>
       </c>
@@ -7274,7 +7275,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>423</v>
       </c>
@@ -7300,7 +7301,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>428</v>
       </c>
@@ -7326,7 +7327,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>433</v>
       </c>
@@ -7352,7 +7353,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>438</v>
       </c>
@@ -7378,7 +7379,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>445</v>
       </c>
@@ -7404,7 +7405,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>449</v>
       </c>
@@ -7430,7 +7431,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>453</v>
       </c>
@@ -7456,7 +7457,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>459</v>
       </c>
@@ -7482,7 +7483,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>464</v>
       </c>
@@ -7508,7 +7509,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>471</v>
       </c>
@@ -7534,7 +7535,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>477</v>
       </c>
@@ -7560,7 +7561,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>483</v>
       </c>
@@ -7586,7 +7587,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>490</v>
       </c>
@@ -7612,7 +7613,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>497</v>
       </c>
@@ -7638,7 +7639,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>501</v>
       </c>
@@ -7664,7 +7665,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>505</v>
       </c>
@@ -7690,7 +7691,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>511</v>
       </c>
@@ -7716,7 +7717,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>515</v>
       </c>
@@ -7742,7 +7743,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>521</v>
       </c>
@@ -7768,7 +7769,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>526</v>
       </c>
@@ -7794,7 +7795,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>530</v>
       </c>
@@ -7820,7 +7821,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>534</v>
       </c>
@@ -7846,7 +7847,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>538</v>
       </c>
@@ -7872,7 +7873,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>541</v>
       </c>
@@ -7898,7 +7899,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>545</v>
       </c>
@@ -7924,7 +7925,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>549</v>
       </c>
@@ -7950,7 +7951,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>553</v>
       </c>
@@ -7976,7 +7977,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>557</v>
       </c>
@@ -8002,7 +8003,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>561</v>
       </c>
@@ -8028,7 +8029,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>565</v>
       </c>
@@ -8054,7 +8055,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>568</v>
       </c>
@@ -8080,7 +8081,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>572</v>
       </c>
@@ -8106,7 +8107,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>576</v>
       </c>
@@ -8132,7 +8133,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>580</v>
       </c>
@@ -8158,7 +8159,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>583</v>
       </c>
@@ -8184,7 +8185,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>586</v>
       </c>
@@ -8210,7 +8211,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>590</v>
       </c>
@@ -8236,7 +8237,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>595</v>
       </c>
@@ -8262,7 +8263,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>600</v>
       </c>
@@ -8288,7 +8289,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>606</v>
       </c>
@@ -8314,7 +8315,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>610</v>
       </c>
@@ -8340,7 +8341,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>616</v>
       </c>
@@ -8366,7 +8367,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>621</v>
       </c>
@@ -8392,7 +8393,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>625</v>
       </c>
@@ -8418,7 +8419,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>628</v>
       </c>
@@ -8444,7 +8445,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>632</v>
       </c>
@@ -8470,7 +8471,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>636</v>
       </c>
@@ -8496,7 +8497,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>640</v>
       </c>
@@ -8522,7 +8523,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>646</v>
       </c>
@@ -8548,7 +8549,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>650</v>
       </c>
@@ -8574,7 +8575,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>654</v>
       </c>
@@ -8600,7 +8601,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>657</v>
       </c>
@@ -8626,7 +8627,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>663</v>
       </c>
@@ -8652,7 +8653,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>666</v>
       </c>
@@ -8678,7 +8679,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>671</v>
       </c>
@@ -8704,7 +8705,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>675</v>
       </c>
@@ -8730,7 +8731,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>678</v>
       </c>
@@ -8756,7 +8757,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>682</v>
       </c>
@@ -8782,7 +8783,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>685</v>
       </c>
@@ -8808,7 +8809,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>688</v>
       </c>
@@ -8834,7 +8835,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>693</v>
       </c>
@@ -8860,7 +8861,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>697</v>
       </c>
@@ -8886,7 +8887,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>700</v>
       </c>
@@ -8912,7 +8913,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>706</v>
       </c>
@@ -8938,7 +8939,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>709</v>
       </c>
@@ -8964,7 +8965,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>712</v>
       </c>
@@ -8990,7 +8991,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>717</v>
       </c>
@@ -9016,7 +9017,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>720</v>
       </c>
@@ -9042,7 +9043,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>724</v>
       </c>
@@ -9068,7 +9069,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>728</v>
       </c>
@@ -9094,7 +9095,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>732</v>
       </c>
@@ -9120,7 +9121,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>735</v>
       </c>
@@ -9146,7 +9147,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>738</v>
       </c>
@@ -9172,7 +9173,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>742</v>
       </c>
@@ -9198,7 +9199,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>746</v>
       </c>
@@ -9224,7 +9225,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>749</v>
       </c>
@@ -9250,7 +9251,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>753</v>
       </c>
@@ -9276,7 +9277,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>760</v>
       </c>
@@ -9302,7 +9303,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>763</v>
       </c>
@@ -9328,7 +9329,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>766</v>
       </c>
@@ -9354,7 +9355,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>770</v>
       </c>
@@ -9380,7 +9381,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>774</v>
       </c>
@@ -9406,7 +9407,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>778</v>
       </c>
@@ -9432,7 +9433,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>783</v>
       </c>
@@ -9458,7 +9459,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>787</v>
       </c>
@@ -9484,7 +9485,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>793</v>
       </c>
@@ -9510,7 +9511,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>800</v>
       </c>
@@ -9536,7 +9537,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>806</v>
       </c>
@@ -9562,7 +9563,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>809</v>
       </c>
@@ -9588,7 +9589,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>813</v>
       </c>
@@ -9614,7 +9615,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>816</v>
       </c>
@@ -9640,7 +9641,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>819</v>
       </c>
@@ -9666,7 +9667,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>823</v>
       </c>
@@ -9692,7 +9693,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>828</v>
       </c>
@@ -9718,7 +9719,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>835</v>
       </c>
@@ -9744,7 +9745,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>838</v>
       </c>
@@ -9770,7 +9771,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>841</v>
       </c>
@@ -9796,7 +9797,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>844</v>
       </c>
@@ -9822,7 +9823,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>848</v>
       </c>
@@ -9848,7 +9849,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>851</v>
       </c>
@@ -9874,7 +9875,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>857</v>
       </c>
@@ -9900,7 +9901,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>860</v>
       </c>
@@ -9926,7 +9927,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>866</v>
       </c>
@@ -9952,7 +9953,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>874</v>
       </c>
@@ -9978,7 +9979,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>877</v>
       </c>
@@ -10004,7 +10005,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>880</v>
       </c>
@@ -10030,7 +10031,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>884</v>
       </c>
@@ -10056,7 +10057,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>888</v>
       </c>
@@ -10082,7 +10083,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>893</v>
       </c>
@@ -10108,7 +10109,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>896</v>
       </c>
@@ -10134,7 +10135,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>899</v>
       </c>
@@ -10160,7 +10161,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>902</v>
       </c>
@@ -10186,7 +10187,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>906</v>
       </c>
@@ -10212,7 +10213,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>909</v>
       </c>
@@ -10238,7 +10239,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>912</v>
       </c>
@@ -10264,7 +10265,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>917</v>
       </c>
@@ -10290,7 +10291,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>920</v>
       </c>
@@ -10316,7 +10317,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>923</v>
       </c>
@@ -10342,7 +10343,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>926</v>
       </c>
@@ -10368,7 +10369,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>929</v>
       </c>
@@ -10394,7 +10395,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>933</v>
       </c>
@@ -10420,7 +10421,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>937</v>
       </c>
@@ -10446,7 +10447,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>941</v>
       </c>
@@ -10472,7 +10473,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>945</v>
       </c>
@@ -10498,7 +10499,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>949</v>
       </c>
@@ -10524,7 +10525,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>952</v>
       </c>
@@ -10550,7 +10551,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>955</v>
       </c>
@@ -10576,7 +10577,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
         <v>960</v>
       </c>
@@ -10602,7 +10603,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>963</v>
       </c>
@@ -10628,7 +10629,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>966</v>
       </c>
@@ -10654,7 +10655,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>969</v>
       </c>
@@ -10680,7 +10681,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>972</v>
       </c>
@@ -10706,7 +10707,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>977</v>
       </c>
@@ -10732,7 +10733,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>980</v>
       </c>
@@ -10758,7 +10759,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>982</v>
       </c>
@@ -10784,7 +10785,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
         <v>985</v>
       </c>
@@ -10810,7 +10811,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
         <v>988</v>
       </c>
@@ -10836,7 +10837,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
         <v>991</v>
       </c>
@@ -10862,7 +10863,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>995</v>
       </c>
@@ -10888,7 +10889,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
         <v>1002</v>
       </c>
@@ -10914,7 +10915,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>1007</v>
       </c>
@@ -10940,7 +10941,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
         <v>1010</v>
       </c>
@@ -10966,7 +10967,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
         <v>1013</v>
       </c>
@@ -10992,7 +10993,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
         <v>1016</v>
       </c>
@@ -11018,7 +11019,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
         <v>1019</v>
       </c>
@@ -11044,7 +11045,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
         <v>1022</v>
       </c>
@@ -11070,7 +11071,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>1025</v>
       </c>
@@ -11096,7 +11097,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
         <v>1028</v>
       </c>
@@ -11122,7 +11123,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>1032</v>
       </c>
@@ -11148,7 +11149,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>1035</v>
       </c>
@@ -11174,7 +11175,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>1038</v>
       </c>
@@ -11200,7 +11201,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
         <v>1042</v>
       </c>
@@ -11226,7 +11227,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
         <v>1045</v>
       </c>
@@ -11252,7 +11253,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
         <v>1048</v>
       </c>
@@ -11278,7 +11279,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>1050</v>
       </c>
@@ -11304,7 +11305,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
         <v>1053</v>
       </c>
@@ -11330,7 +11331,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>1057</v>
       </c>
@@ -11356,7 +11357,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
         <v>1060</v>
       </c>
@@ -11382,7 +11383,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>1063</v>
       </c>
@@ -11408,7 +11409,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
         <v>1066</v>
       </c>
@@ -11434,7 +11435,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
         <v>1069</v>
       </c>
@@ -11460,7 +11461,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
         <v>1072</v>
       </c>
@@ -11486,7 +11487,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
         <v>1075</v>
       </c>
@@ -11512,7 +11513,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
         <v>1081</v>
       </c>
@@ -11538,7 +11539,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
         <v>1085</v>
       </c>
@@ -11564,7 +11565,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
         <v>1090</v>
       </c>
@@ -11590,7 +11591,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>1093</v>
       </c>
@@ -11616,7 +11617,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
         <v>1097</v>
       </c>
@@ -11642,7 +11643,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
         <v>1100</v>
       </c>
@@ -11668,7 +11669,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
         <v>1103</v>
       </c>
@@ -11694,7 +11695,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
         <v>1106</v>
       </c>
@@ -11720,7 +11721,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
         <v>1109</v>
       </c>
@@ -11746,7 +11747,7 @@
         <v>1114</v>
       </c>
     </row>
-    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
         <v>1115</v>
       </c>
@@ -11772,7 +11773,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="245" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
         <v>1119</v>
       </c>
@@ -11798,7 +11799,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
         <v>1122</v>
       </c>
@@ -11824,7 +11825,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="247" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
         <v>1125</v>
       </c>
@@ -11850,7 +11851,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
         <v>1128</v>
       </c>
@@ -11876,7 +11877,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
         <v>1131</v>
       </c>
@@ -11902,7 +11903,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
         <v>1134</v>
       </c>
@@ -11928,7 +11929,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="251" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
         <v>1137</v>
       </c>
@@ -11954,7 +11955,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>1141</v>
       </c>
@@ -11980,7 +11981,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="253" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
         <v>1144</v>
       </c>
@@ -12006,7 +12007,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="254" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
         <v>1147</v>
       </c>
@@ -12032,7 +12033,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="255" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
         <v>1150</v>
       </c>
@@ -12058,7 +12059,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="256" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
         <v>1153</v>
       </c>
@@ -12084,7 +12085,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="257" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
         <v>1156</v>
       </c>
@@ -12110,7 +12111,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="258" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
         <v>1159</v>
       </c>
@@ -12136,7 +12137,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="259" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
         <v>1162</v>
       </c>
@@ -12162,7 +12163,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="260" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
         <v>1165</v>
       </c>
@@ -12188,7 +12189,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="261" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
         <v>1168</v>
       </c>
@@ -12214,7 +12215,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="262" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
         <v>1171</v>
       </c>
@@ -12240,7 +12241,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="263" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
         <v>1173</v>
       </c>
@@ -12266,7 +12267,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="264" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
         <v>1175</v>
       </c>
@@ -12292,7 +12293,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="265" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
         <v>1178</v>
       </c>
@@ -12318,7 +12319,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="266" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
         <v>1181</v>
       </c>
@@ -12344,7 +12345,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="267" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
         <v>1184</v>
       </c>
@@ -12370,7 +12371,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="268" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
         <v>1187</v>
       </c>
@@ -12396,7 +12397,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="269" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
         <v>1190</v>
       </c>
@@ -12422,7 +12423,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="270" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
         <v>1193</v>
       </c>
@@ -12448,7 +12449,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="271" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
         <v>1198</v>
       </c>
@@ -12474,7 +12475,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="272" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
         <v>1202</v>
       </c>
@@ -12500,7 +12501,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="273" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
         <v>1205</v>
       </c>
@@ -12526,7 +12527,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="274" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
         <v>1208</v>
       </c>
@@ -12552,7 +12553,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
         <v>1212</v>
       </c>
@@ -12578,7 +12579,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
         <v>1216</v>
       </c>
@@ -12604,7 +12605,7 @@
         <v>1219</v>
       </c>
     </row>
-    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
         <v>1220</v>
       </c>
@@ -12630,7 +12631,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="278" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
         <v>1223</v>
       </c>
@@ -12656,7 +12657,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="279" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
         <v>1227</v>
       </c>
@@ -12682,7 +12683,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="280" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
         <v>1230</v>
       </c>
@@ -12708,7 +12709,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="281" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
         <v>1233</v>
       </c>
@@ -12734,7 +12735,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="282" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
         <v>1236</v>
       </c>
@@ -12760,7 +12761,7 @@
         <v>1241</v>
       </c>
     </row>
-    <row r="283" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
         <v>1242</v>
       </c>
@@ -12786,7 +12787,7 @@
         <v>1248</v>
       </c>
     </row>
-    <row r="284" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
         <v>1249</v>
       </c>
@@ -12812,7 +12813,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="285" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
         <v>1253</v>
       </c>
@@ -12838,7 +12839,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="286" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
         <v>1257</v>
       </c>
@@ -12864,7 +12865,7 @@
         <v>1261</v>
       </c>
     </row>
-    <row r="287" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
         <v>1262</v>
       </c>
@@ -12890,7 +12891,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="288" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
         <v>1266</v>
       </c>
@@ -12916,7 +12917,7 @@
         <v>1272</v>
       </c>
     </row>
-    <row r="289" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
         <v>1273</v>
       </c>
@@ -12942,7 +12943,7 @@
         <v>1277</v>
       </c>
     </row>
-    <row r="290" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
         <v>1278</v>
       </c>
@@ -12968,7 +12969,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="291" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
         <v>1282</v>
       </c>
@@ -12994,7 +12995,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="292" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
         <v>1285</v>
       </c>
@@ -13020,7 +13021,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="293" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
         <v>1288</v>
       </c>
@@ -13046,7 +13047,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="294" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
         <v>1291</v>
       </c>
@@ -13072,7 +13073,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="295" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
         <v>1295</v>
       </c>
@@ -13098,7 +13099,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="296" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
         <v>1299</v>
       </c>
@@ -13124,7 +13125,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="297" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
         <v>1302</v>
       </c>
@@ -13150,7 +13151,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="298" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
         <v>1305</v>
       </c>
@@ -13176,7 +13177,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="299" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
         <v>1308</v>
       </c>
@@ -13202,7 +13203,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="300" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300" s="1" t="s">
         <v>1311</v>
       </c>
@@ -13228,7 +13229,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="301" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301" s="1" t="s">
         <v>1314</v>
       </c>
@@ -13254,7 +13255,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="302" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302" s="1" t="s">
         <v>1317</v>
       </c>
@@ -13280,7 +13281,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="303" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303" s="1" t="s">
         <v>1320</v>
       </c>
@@ -13306,7 +13307,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="304" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304" s="1" t="s">
         <v>1323</v>
       </c>
@@ -13332,7 +13333,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="305" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305" s="1" t="s">
         <v>1329</v>
       </c>
@@ -13358,7 +13359,7 @@
         <v>1333</v>
       </c>
     </row>
-    <row r="306" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306" s="1" t="s">
         <v>1334</v>
       </c>
@@ -13384,7 +13385,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="307" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307" s="1" t="s">
         <v>1337</v>
       </c>
@@ -13410,7 +13411,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="308" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308" s="1" t="s">
         <v>1340</v>
       </c>
@@ -13436,7 +13437,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="309" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309" s="1" t="s">
         <v>1344</v>
       </c>
@@ -13462,7 +13463,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="310" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310" s="1" t="s">
         <v>1347</v>
       </c>
@@ -13488,7 +13489,7 @@
         <v>1352</v>
       </c>
     </row>
-    <row r="311" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311" s="1" t="s">
         <v>1353</v>
       </c>
@@ -13514,7 +13515,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="312" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312" s="1" t="s">
         <v>1357</v>
       </c>
@@ -13540,7 +13541,7 @@
         <v>1197</v>
       </c>
     </row>
-    <row r="313" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313" s="1" t="s">
         <v>1362</v>
       </c>
@@ -13566,7 +13567,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="314" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314" s="1" t="s">
         <v>1365</v>
       </c>
@@ -13592,7 +13593,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="315" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315" s="1" t="s">
         <v>1368</v>
       </c>
@@ -13618,7 +13619,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="316" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316" s="1" t="s">
         <v>1372</v>
       </c>
@@ -13644,7 +13645,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="317" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317" s="1" t="s">
         <v>1375</v>
       </c>
@@ -13670,7 +13671,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="318" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318" s="1" t="s">
         <v>1378</v>
       </c>
@@ -13696,7 +13697,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="319" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A319" s="1" t="s">
         <v>1382</v>
       </c>
@@ -13722,7 +13723,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="320" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A320" s="1" t="s">
         <v>1385</v>
       </c>
@@ -13748,7 +13749,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="321" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321" s="1" t="s">
         <v>1388</v>
       </c>
@@ -13774,7 +13775,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="322" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322" s="1" t="s">
         <v>1391</v>
       </c>
@@ -13800,7 +13801,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="323" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A323" s="1" t="s">
         <v>1394</v>
       </c>
@@ -13826,7 +13827,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="324" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A324" s="1" t="s">
         <v>1397</v>
       </c>
@@ -13852,7 +13853,7 @@
         <v>1402</v>
       </c>
     </row>
-    <row r="325" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325" s="1" t="s">
         <v>1403</v>
       </c>
@@ -13878,7 +13879,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="326" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326" s="1" t="s">
         <v>1405</v>
       </c>
@@ -13904,7 +13905,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="327" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A327" s="1" t="s">
         <v>1408</v>
       </c>
@@ -13930,7 +13931,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="328" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328" s="1" t="s">
         <v>1411</v>
       </c>
@@ -13956,7 +13957,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="329" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A329" s="1" t="s">
         <v>1414</v>
       </c>
@@ -13982,7 +13983,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="330" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A330" s="1" t="s">
         <v>1417</v>
       </c>
@@ -14008,7 +14009,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="331" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A331" s="1" t="s">
         <v>1421</v>
       </c>
@@ -14034,7 +14035,7 @@
         <v>1096</v>
       </c>
     </row>
-    <row r="332" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A332" s="1" t="s">
         <v>1425</v>
       </c>
@@ -14060,7 +14061,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="333" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A333" s="1" t="s">
         <v>1428</v>
       </c>
@@ -14086,7 +14087,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="334" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A334" s="1" t="s">
         <v>1431</v>
       </c>
@@ -14112,7 +14113,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="335" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A335" s="1" t="s">
         <v>1435</v>
       </c>
@@ -14138,7 +14139,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="336" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336" s="1" t="s">
         <v>1438</v>
       </c>
@@ -14164,7 +14165,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="337" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A337" s="1" t="s">
         <v>1441</v>
       </c>
@@ -14190,7 +14191,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="338" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338" s="1" t="s">
         <v>1444</v>
       </c>
@@ -14216,7 +14217,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="339" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A339" s="1" t="s">
         <v>1446</v>
       </c>
@@ -14242,7 +14243,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="340" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A340" s="1" t="s">
         <v>1449</v>
       </c>
@@ -14268,7 +14269,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="341" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A341" s="1" t="s">
         <v>1452</v>
       </c>
@@ -14294,7 +14295,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="342" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A342" s="1" t="s">
         <v>1457</v>
       </c>
@@ -14320,7 +14321,7 @@
         <v>1462</v>
       </c>
     </row>
-    <row r="343" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A343" s="1" t="s">
         <v>1463</v>
       </c>
@@ -14346,7 +14347,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="344" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344" s="1" t="s">
         <v>1466</v>
       </c>
@@ -14372,7 +14373,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="345" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A345" s="1" t="s">
         <v>1469</v>
       </c>
@@ -14398,7 +14399,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="346" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A346" s="1" t="s">
         <v>1471</v>
       </c>
@@ -14424,7 +14425,7 @@
         <v>1475</v>
       </c>
     </row>
-    <row r="347" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A347" s="1" t="s">
         <v>1476</v>
       </c>
@@ -14450,7 +14451,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="348" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348" s="1" t="s">
         <v>1479</v>
       </c>
@@ -14476,7 +14477,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="349" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A349" s="1" t="s">
         <v>1483</v>
       </c>
@@ -14502,7 +14503,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="350" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A350" s="1" t="s">
         <v>1486</v>
       </c>
@@ -14528,7 +14529,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="351" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A351" s="1" t="s">
         <v>1489</v>
       </c>
@@ -14554,7 +14555,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="352" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A352" s="1" t="s">
         <v>1492</v>
       </c>
@@ -14580,7 +14581,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="353" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A353" s="1" t="s">
         <v>1496</v>
       </c>
@@ -14606,7 +14607,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="354" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A354" s="1" t="s">
         <v>1498</v>
       </c>
@@ -14632,7 +14633,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="355" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A355" s="1" t="s">
         <v>1501</v>
       </c>
@@ -14658,7 +14659,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="356" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A356" s="1" t="s">
         <v>1504</v>
       </c>
@@ -14684,7 +14685,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="357" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A357" s="1" t="s">
         <v>1508</v>
       </c>
@@ -14710,7 +14711,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="358" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A358" s="1" t="s">
         <v>1511</v>
       </c>
@@ -14736,7 +14737,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="359" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A359" s="1" t="s">
         <v>1514</v>
       </c>
@@ -14762,7 +14763,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="360" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A360" s="1" t="s">
         <v>1517</v>
       </c>
@@ -14788,7 +14789,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="361" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A361" s="1" t="s">
         <v>1522</v>
       </c>
@@ -14814,7 +14815,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="362" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A362" s="1" t="s">
         <v>1525</v>
       </c>
@@ -14840,7 +14841,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="363" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A363" s="1" t="s">
         <v>1528</v>
       </c>
@@ -14866,7 +14867,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="364" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A364" s="1" t="s">
         <v>1531</v>
       </c>
@@ -14892,7 +14893,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="365" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A365" s="1" t="s">
         <v>1534</v>
       </c>
@@ -14918,7 +14919,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="366" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A366" s="1" t="s">
         <v>1536</v>
       </c>
@@ -14944,7 +14945,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="367" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A367" s="1" t="s">
         <v>1540</v>
       </c>
@@ -14970,7 +14971,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="368" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A368" s="1" t="s">
         <v>1543</v>
       </c>
@@ -14996,7 +14997,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="369" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A369" s="1" t="s">
         <v>1546</v>
       </c>
@@ -15022,7 +15023,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="370" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A370" s="1" t="s">
         <v>1549</v>
       </c>
@@ -15048,7 +15049,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="371" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A371" s="1" t="s">
         <v>1552</v>
       </c>
@@ -15074,7 +15075,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="372" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A372" s="1" t="s">
         <v>1555</v>
       </c>
@@ -15100,7 +15101,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="373" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A373" s="1" t="s">
         <v>1559</v>
       </c>
@@ -15126,7 +15127,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="374" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A374" s="1" t="s">
         <v>1562</v>
       </c>
@@ -15152,7 +15153,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="375" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A375" s="1" t="s">
         <v>1565</v>
       </c>
@@ -15178,7 +15179,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="376" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A376" s="1" t="s">
         <v>1569</v>
       </c>
@@ -15204,7 +15205,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="377" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A377" s="1" t="s">
         <v>1572</v>
       </c>
@@ -15230,7 +15231,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="378" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A378" s="1" t="s">
         <v>1575</v>
       </c>
@@ -15256,7 +15257,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="379" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A379" s="1" t="s">
         <v>1578</v>
       </c>
@@ -15282,7 +15283,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="380" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A380" s="1" t="s">
         <v>1582</v>
       </c>
@@ -15308,7 +15309,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="381" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A381" s="1" t="s">
         <v>1585</v>
       </c>
@@ -15334,7 +15335,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="382" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A382" s="1" t="s">
         <v>1588</v>
       </c>
@@ -15360,7 +15361,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="383" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A383" s="1" t="s">
         <v>1591</v>
       </c>
@@ -15386,7 +15387,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="384" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A384" s="1" t="s">
         <v>1594</v>
       </c>
@@ -15412,7 +15413,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="385" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A385" s="1" t="s">
         <v>1597</v>
       </c>
@@ -15438,7 +15439,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="386" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A386" s="1" t="s">
         <v>1600</v>
       </c>
@@ -15464,7 +15465,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="387" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A387" s="1" t="s">
         <v>1604</v>
       </c>
@@ -15490,7 +15491,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="388" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A388" s="1" t="s">
         <v>1607</v>
       </c>
@@ -15516,7 +15517,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="389" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A389" s="1" t="s">
         <v>1610</v>
       </c>
@@ -15542,7 +15543,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="390" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A390" s="1" t="s">
         <v>1613</v>
       </c>
@@ -15568,7 +15569,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="391" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A391" s="1" t="s">
         <v>1616</v>
       </c>
@@ -15594,7 +15595,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="392" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A392" s="1" t="s">
         <v>1619</v>
       </c>
@@ -15620,7 +15621,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="393" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A393" s="1" t="s">
         <v>1622</v>
       </c>
@@ -15646,7 +15647,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="394" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A394" s="1" t="s">
         <v>1625</v>
       </c>
@@ -15672,7 +15673,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="395" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A395" s="1" t="s">
         <v>1628</v>
       </c>
@@ -15698,7 +15699,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="396" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A396" s="1" t="s">
         <v>1631</v>
       </c>
@@ -15724,7 +15725,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="397" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A397" s="1" t="s">
         <v>1634</v>
       </c>
@@ -15750,7 +15751,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="398" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A398" s="1" t="s">
         <v>1637</v>
       </c>
@@ -15776,7 +15777,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="399" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A399" s="1" t="s">
         <v>1640</v>
       </c>
@@ -15802,7 +15803,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="400" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A400" s="1" t="s">
         <v>1643</v>
       </c>
@@ -15828,7 +15829,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="401" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A401" s="1" t="s">
         <v>1647</v>
       </c>
@@ -15854,7 +15855,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="402" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A402" s="1" t="s">
         <v>1650</v>
       </c>
@@ -15907,7 +15908,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:H2" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A2:H403" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="State Totals"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="A1:H1"/>
   </mergeCells>

</xml_diff>